<commit_message>
Added analytics and move valiator duplicate to All records data
</commit_message>
<xml_diff>
--- a/Duplicate_Transactions.xlsx
+++ b/Duplicate_Transactions.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N73"/>
+  <dimension ref="A1:N84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4070,10 +4070,8 @@
           <t>Gurinder Singh Aulakh</t>
         </is>
       </c>
-      <c r="B73" t="inlineStr">
-        <is>
-          <t>12096508105</t>
-        </is>
+      <c r="B73" t="n">
+        <v>12096508105</v>
       </c>
       <c r="C73" t="inlineStr">
         <is>
@@ -4116,6 +4114,559 @@
         </is>
       </c>
     </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>Madhukar Verma</t>
+        </is>
+      </c>
+      <c r="B74" t="n">
+        <v>2065044242</v>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>42729 Mayfair Park Ave Fremont Fremont 94538 California USA</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>JKR</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>English</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr"/>
+      <c r="G74" t="inlineStr"/>
+      <c r="H74" t="inlineStr"/>
+      <c r="I74" t="inlineStr"/>
+      <c r="J74" t="inlineStr"/>
+      <c r="K74" t="inlineStr">
+        <is>
+          <t>Same book already sent</t>
+        </is>
+      </c>
+      <c r="L74" t="inlineStr">
+        <is>
+          <t>2025-09-15 16:36:51</t>
+        </is>
+      </c>
+      <c r="M74" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="N74" t="inlineStr">
+        <is>
+          <t>Blocked</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>Fnu Balan</t>
+        </is>
+      </c>
+      <c r="B75" t="n">
+        <v>2065044242</v>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>202 Hovis Rd Hovis Rd 28164 Nc USA</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>JKR</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>English</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr"/>
+      <c r="G75" t="inlineStr"/>
+      <c r="H75" t="inlineStr"/>
+      <c r="I75" t="inlineStr"/>
+      <c r="J75" t="inlineStr"/>
+      <c r="K75" t="inlineStr">
+        <is>
+          <t>Same book already sent</t>
+        </is>
+      </c>
+      <c r="L75" t="inlineStr">
+        <is>
+          <t>2025-09-15 16:36:57</t>
+        </is>
+      </c>
+      <c r="M75" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="N75" t="inlineStr">
+        <is>
+          <t>Blocked</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>Amanda Father - Vazquez</t>
+        </is>
+      </c>
+      <c r="B76" t="n">
+        <v>2065044242</v>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>116 cypress Vallejo Ca 94590 United States</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>English</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr"/>
+      <c r="G76" t="inlineStr"/>
+      <c r="H76" t="inlineStr"/>
+      <c r="I76" t="inlineStr"/>
+      <c r="J76" t="inlineStr"/>
+      <c r="K76" t="inlineStr">
+        <is>
+          <t>Same book already sent</t>
+        </is>
+      </c>
+      <c r="L76" t="inlineStr">
+        <is>
+          <t>2025-09-15 16:36:59</t>
+        </is>
+      </c>
+      <c r="M76" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="N76" t="inlineStr">
+        <is>
+          <t>Blocked</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>Thomas Schenck</t>
+        </is>
+      </c>
+      <c r="B77" t="n">
+        <v>2065044242</v>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>408 210 5th avenue south Saint Petersburg 33701 Florida United States</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>English</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr"/>
+      <c r="G77" t="inlineStr"/>
+      <c r="H77" t="inlineStr"/>
+      <c r="I77" t="inlineStr"/>
+      <c r="J77" t="inlineStr"/>
+      <c r="K77" t="inlineStr">
+        <is>
+          <t>Same book already sent</t>
+        </is>
+      </c>
+      <c r="L77" t="inlineStr">
+        <is>
+          <t>2025-09-15 16:37:01</t>
+        </is>
+      </c>
+      <c r="M77" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="N77" t="inlineStr">
+        <is>
+          <t>Blocked</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>Atha Bass</t>
+        </is>
+      </c>
+      <c r="B78" t="n">
+        <v>2065044242</v>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>202 10404 Salvia Street, Charlotte, 28277, North Carolina, USA</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>JKR</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>English</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr"/>
+      <c r="G78" t="inlineStr"/>
+      <c r="H78" t="inlineStr"/>
+      <c r="I78" t="inlineStr"/>
+      <c r="J78" t="inlineStr"/>
+      <c r="K78" t="inlineStr">
+        <is>
+          <t>Same book already sent</t>
+        </is>
+      </c>
+      <c r="L78" t="inlineStr">
+        <is>
+          <t>2025-09-15 16:37:08</t>
+        </is>
+      </c>
+      <c r="M78" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="N78" t="inlineStr">
+        <is>
+          <t>Blocked</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>Thyagarajan Iyer</t>
+        </is>
+      </c>
+      <c r="B79" t="n">
+        <v>2065044242</v>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>6092 Elmbridge Dr, San Jose, 95129, CA, USA</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>JKR</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>English</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr"/>
+      <c r="G79" t="inlineStr"/>
+      <c r="H79" t="inlineStr"/>
+      <c r="I79" t="inlineStr"/>
+      <c r="J79" t="inlineStr"/>
+      <c r="K79" t="inlineStr">
+        <is>
+          <t>Same book already sent</t>
+        </is>
+      </c>
+      <c r="L79" t="inlineStr">
+        <is>
+          <t>2025-09-15 16:37:10</t>
+        </is>
+      </c>
+      <c r="M79" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="N79" t="inlineStr">
+        <is>
+          <t>Blocked</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>Janakkumar Babulal</t>
+        </is>
+      </c>
+      <c r="B80" t="n">
+        <v>2065044242</v>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>3220 1st Street, Rosenberg, Fort Bend, TX 77471, USA</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>Gujarati</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr"/>
+      <c r="G80" t="inlineStr"/>
+      <c r="H80" t="inlineStr"/>
+      <c r="I80" t="inlineStr"/>
+      <c r="J80" t="inlineStr"/>
+      <c r="K80" t="inlineStr">
+        <is>
+          <t>Same book already sent</t>
+        </is>
+      </c>
+      <c r="L80" t="inlineStr">
+        <is>
+          <t>2025-09-15 16:37:12</t>
+        </is>
+      </c>
+      <c r="M80" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="N80" t="inlineStr">
+        <is>
+          <t>Blocked</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>Janakkumar Babulal</t>
+        </is>
+      </c>
+      <c r="B81" t="n">
+        <v>9165478955</v>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>3220 1st Street, Rosenberg, Fort Bend, TX 77471, USA</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>Gujarati</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr"/>
+      <c r="G81" t="inlineStr"/>
+      <c r="H81" t="inlineStr"/>
+      <c r="I81" t="inlineStr"/>
+      <c r="J81" t="inlineStr"/>
+      <c r="K81" t="inlineStr">
+        <is>
+          <t>Same book already sent</t>
+        </is>
+      </c>
+      <c r="L81" t="inlineStr">
+        <is>
+          <t>2025-09-15 16:37:14</t>
+        </is>
+      </c>
+      <c r="M81" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="N81" t="inlineStr">
+        <is>
+          <t>Blocked</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>Jatinder Das</t>
+        </is>
+      </c>
+      <c r="B82" t="n">
+        <v>12096891489</v>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>2027 Westmora ave.
+Stockton, CA 95210</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>YBB</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>Nan</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr"/>
+      <c r="G82" t="inlineStr"/>
+      <c r="H82" t="inlineStr"/>
+      <c r="I82" t="inlineStr"/>
+      <c r="J82" t="inlineStr"/>
+      <c r="K82" t="inlineStr">
+        <is>
+          <t>Same book already sent</t>
+        </is>
+      </c>
+      <c r="L82" t="inlineStr">
+        <is>
+          <t>2025-09-15 16:37:16</t>
+        </is>
+      </c>
+      <c r="M82" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="N82" t="inlineStr">
+        <is>
+          <t>Blocked</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>Gurinder Singh Aulakh</t>
+        </is>
+      </c>
+      <c r="B83" t="n">
+        <v>12096508105</v>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>698 N Plumas Dr, Mountain House, CA 95391</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>JKR</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>Punjabi</t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr"/>
+      <c r="G83" t="inlineStr"/>
+      <c r="H83" t="inlineStr"/>
+      <c r="I83" t="inlineStr"/>
+      <c r="J83" t="inlineStr"/>
+      <c r="K83" t="inlineStr">
+        <is>
+          <t>Same book already sent</t>
+        </is>
+      </c>
+      <c r="L83" t="inlineStr">
+        <is>
+          <t>2025-09-15 16:37:18</t>
+        </is>
+      </c>
+      <c r="M83" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="N83" t="inlineStr">
+        <is>
+          <t>Blocked</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>Sandipkumar Bhupendralal Kapadia</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>2063260971</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>605 West Third Street, Donalsonville, Georgia, 39845, USA</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>Gujarati</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr"/>
+      <c r="G84" t="inlineStr"/>
+      <c r="H84" t="inlineStr"/>
+      <c r="I84" t="inlineStr"/>
+      <c r="J84" t="inlineStr"/>
+      <c r="K84" t="inlineStr">
+        <is>
+          <t>Same book already sent</t>
+        </is>
+      </c>
+      <c r="L84" t="inlineStr">
+        <is>
+          <t>2025-09-15 16:37:21</t>
+        </is>
+      </c>
+      <c r="M84" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="N84" t="inlineStr">
+        <is>
+          <t>Blocked</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Now sending the repated message
</commit_message>
<xml_diff>
--- a/Duplicate_Transactions.xlsx
+++ b/Duplicate_Transactions.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N231"/>
+  <dimension ref="A1:N238"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11978,10 +11978,8 @@
           <t>Madhukar Verma</t>
         </is>
       </c>
-      <c r="B231" t="inlineStr">
-        <is>
-          <t>2065044242</t>
-        </is>
+      <c r="B231" t="n">
+        <v>2065044242</v>
       </c>
       <c r="C231" t="inlineStr">
         <is>
@@ -12024,6 +12022,358 @@
         </is>
       </c>
     </row>
+    <row r="232">
+      <c r="A232" t="inlineStr">
+        <is>
+          <t>David</t>
+        </is>
+      </c>
+      <c r="B232" t="n">
+        <v>12814104622</v>
+      </c>
+      <c r="C232" t="inlineStr">
+        <is>
+          <t>PO Box 87301, Park Place, Houston, Texas</t>
+        </is>
+      </c>
+      <c r="D232" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="E232" t="inlineStr">
+        <is>
+          <t>Po Box 87301, Park Place, Houston, Texas</t>
+        </is>
+      </c>
+      <c r="F232" t="inlineStr"/>
+      <c r="G232" t="inlineStr"/>
+      <c r="H232" t="inlineStr"/>
+      <c r="I232" t="inlineStr"/>
+      <c r="J232" t="inlineStr"/>
+      <c r="K232" t="inlineStr">
+        <is>
+          <t>Same book already sent</t>
+        </is>
+      </c>
+      <c r="L232" t="inlineStr">
+        <is>
+          <t>2025-09-16 13:54:29</t>
+        </is>
+      </c>
+      <c r="M232" t="inlineStr">
+        <is>
+          <t>2025-09-16</t>
+        </is>
+      </c>
+      <c r="N232" t="inlineStr">
+        <is>
+          <t>Blocked</t>
+        </is>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="inlineStr">
+        <is>
+          <t>Henry Chelegbor</t>
+        </is>
+      </c>
+      <c r="B233" t="n">
+        <v>13024705411</v>
+      </c>
+      <c r="C233" t="inlineStr">
+        <is>
+          <t>6613 Guyer Street, Philadelphia, PA, Pennsylvania</t>
+        </is>
+      </c>
+      <c r="D233" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="E233" t="inlineStr">
+        <is>
+          <t>6613 Guyer Street, Philadelphia, Pa, Pennsylvania</t>
+        </is>
+      </c>
+      <c r="F233" t="inlineStr"/>
+      <c r="G233" t="inlineStr"/>
+      <c r="H233" t="inlineStr"/>
+      <c r="I233" t="inlineStr"/>
+      <c r="J233" t="inlineStr"/>
+      <c r="K233" t="inlineStr">
+        <is>
+          <t>Same book already sent</t>
+        </is>
+      </c>
+      <c r="L233" t="inlineStr">
+        <is>
+          <t>2025-09-16 13:54:31</t>
+        </is>
+      </c>
+      <c r="M233" t="inlineStr">
+        <is>
+          <t>2025-09-16</t>
+        </is>
+      </c>
+      <c r="N233" t="inlineStr">
+        <is>
+          <t>Blocked</t>
+        </is>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="inlineStr">
+        <is>
+          <t>Dennis Vanmeter</t>
+        </is>
+      </c>
+      <c r="B234" t="n">
+        <v>13049196111</v>
+      </c>
+      <c r="C234" t="inlineStr">
+        <is>
+          <t>1909 Harper Rd, Beckley, WV 25801</t>
+        </is>
+      </c>
+      <c r="D234" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="E234" t="inlineStr">
+        <is>
+          <t>1909 Harper Rd, Beckley, Wv 25801</t>
+        </is>
+      </c>
+      <c r="F234" t="inlineStr"/>
+      <c r="G234" t="inlineStr"/>
+      <c r="H234" t="inlineStr"/>
+      <c r="I234" t="inlineStr"/>
+      <c r="J234" t="inlineStr"/>
+      <c r="K234" t="inlineStr">
+        <is>
+          <t>Same book already sent</t>
+        </is>
+      </c>
+      <c r="L234" t="inlineStr">
+        <is>
+          <t>2025-09-16 13:54:33</t>
+        </is>
+      </c>
+      <c r="M234" t="inlineStr">
+        <is>
+          <t>2025-09-16</t>
+        </is>
+      </c>
+      <c r="N234" t="inlineStr">
+        <is>
+          <t>Blocked</t>
+        </is>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="inlineStr">
+        <is>
+          <t>Madhukar Verma</t>
+        </is>
+      </c>
+      <c r="B235" t="n">
+        <v>2065044242</v>
+      </c>
+      <c r="C235" t="inlineStr">
+        <is>
+          <t>42729 Mayfair Park Ave Fremont Fremont 94538 California USA</t>
+        </is>
+      </c>
+      <c r="D235" t="inlineStr">
+        <is>
+          <t>YBB</t>
+        </is>
+      </c>
+      <c r="E235" t="inlineStr">
+        <is>
+          <t>English</t>
+        </is>
+      </c>
+      <c r="F235" t="inlineStr"/>
+      <c r="G235" t="inlineStr"/>
+      <c r="H235" t="inlineStr"/>
+      <c r="I235" t="inlineStr"/>
+      <c r="J235" t="inlineStr"/>
+      <c r="K235" t="inlineStr">
+        <is>
+          <t>Same book already sent</t>
+        </is>
+      </c>
+      <c r="L235" t="inlineStr">
+        <is>
+          <t>2025-09-16 13:55:15</t>
+        </is>
+      </c>
+      <c r="M235" t="inlineStr">
+        <is>
+          <t>2025-09-16</t>
+        </is>
+      </c>
+      <c r="N235" t="inlineStr">
+        <is>
+          <t>Blocked</t>
+        </is>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="inlineStr">
+        <is>
+          <t>David</t>
+        </is>
+      </c>
+      <c r="B236" t="n">
+        <v>12814104622</v>
+      </c>
+      <c r="C236" t="inlineStr">
+        <is>
+          <t>PO Box 87301, Park Place, Houston, Texas</t>
+        </is>
+      </c>
+      <c r="D236" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="E236" t="inlineStr">
+        <is>
+          <t>Po Box 87301, Park Place, Houston, Texas</t>
+        </is>
+      </c>
+      <c r="F236" t="inlineStr"/>
+      <c r="G236" t="inlineStr"/>
+      <c r="H236" t="inlineStr"/>
+      <c r="I236" t="inlineStr"/>
+      <c r="J236" t="inlineStr"/>
+      <c r="K236" t="inlineStr">
+        <is>
+          <t>Same book already sent</t>
+        </is>
+      </c>
+      <c r="L236" t="inlineStr">
+        <is>
+          <t>2025-09-16 13:55:17</t>
+        </is>
+      </c>
+      <c r="M236" t="inlineStr">
+        <is>
+          <t>2025-09-16</t>
+        </is>
+      </c>
+      <c r="N236" t="inlineStr">
+        <is>
+          <t>Blocked</t>
+        </is>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="inlineStr">
+        <is>
+          <t>Henry Chelegbor</t>
+        </is>
+      </c>
+      <c r="B237" t="n">
+        <v>13024705411</v>
+      </c>
+      <c r="C237" t="inlineStr">
+        <is>
+          <t>6613 Guyer Street, Philadelphia, PA, Pennsylvania</t>
+        </is>
+      </c>
+      <c r="D237" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="E237" t="inlineStr">
+        <is>
+          <t>6613 Guyer Street, Philadelphia, Pa, Pennsylvania</t>
+        </is>
+      </c>
+      <c r="F237" t="inlineStr"/>
+      <c r="G237" t="inlineStr"/>
+      <c r="H237" t="inlineStr"/>
+      <c r="I237" t="inlineStr"/>
+      <c r="J237" t="inlineStr"/>
+      <c r="K237" t="inlineStr">
+        <is>
+          <t>Same book already sent</t>
+        </is>
+      </c>
+      <c r="L237" t="inlineStr">
+        <is>
+          <t>2025-09-16 13:55:20</t>
+        </is>
+      </c>
+      <c r="M237" t="inlineStr">
+        <is>
+          <t>2025-09-16</t>
+        </is>
+      </c>
+      <c r="N237" t="inlineStr">
+        <is>
+          <t>Blocked</t>
+        </is>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="inlineStr">
+        <is>
+          <t>Dennis Vanmeter</t>
+        </is>
+      </c>
+      <c r="B238" t="inlineStr">
+        <is>
+          <t>13049196111</t>
+        </is>
+      </c>
+      <c r="C238" t="inlineStr">
+        <is>
+          <t>1909 Harper Rd, Beckley, WV 25801</t>
+        </is>
+      </c>
+      <c r="D238" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="E238" t="inlineStr">
+        <is>
+          <t>1909 Harper Rd, Beckley, Wv 25801</t>
+        </is>
+      </c>
+      <c r="F238" t="inlineStr"/>
+      <c r="G238" t="inlineStr"/>
+      <c r="H238" t="inlineStr"/>
+      <c r="I238" t="inlineStr"/>
+      <c r="J238" t="inlineStr"/>
+      <c r="K238" t="inlineStr">
+        <is>
+          <t>Same book already sent</t>
+        </is>
+      </c>
+      <c r="L238" t="inlineStr">
+        <is>
+          <t>2025-09-16 13:55:22</t>
+        </is>
+      </c>
+      <c r="M238" t="inlineStr">
+        <is>
+          <t>2025-09-16</t>
+        </is>
+      </c>
+      <c r="N238" t="inlineStr">
+        <is>
+          <t>Blocked</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Whatsapp and sms bth working now
</commit_message>
<xml_diff>
--- a/Duplicate_Transactions.xlsx
+++ b/Duplicate_Transactions.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N410"/>
+  <dimension ref="A1:N432"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -20928,10 +20928,8 @@
           <t>Madhukar Verma</t>
         </is>
       </c>
-      <c r="B410" t="inlineStr">
-        <is>
-          <t>2065044242</t>
-        </is>
+      <c r="B410" t="n">
+        <v>2065044242</v>
       </c>
       <c r="C410" t="inlineStr">
         <is>
@@ -20974,6 +20972,1108 @@
         </is>
       </c>
     </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>David</t>
+        </is>
+      </c>
+      <c r="B411" t="n">
+        <v>12814104622</v>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>PO Box 87301, Park Place, Houston, Texas</t>
+        </is>
+      </c>
+      <c r="D411" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="E411" t="inlineStr">
+        <is>
+          <t>Po Box 87301, Park Place, Houston, Texas</t>
+        </is>
+      </c>
+      <c r="F411" t="inlineStr"/>
+      <c r="G411" t="inlineStr"/>
+      <c r="H411" t="inlineStr"/>
+      <c r="I411" t="inlineStr"/>
+      <c r="J411" t="inlineStr"/>
+      <c r="K411" t="inlineStr">
+        <is>
+          <t>WhatsApp message already sent for this book previously</t>
+        </is>
+      </c>
+      <c r="L411" t="inlineStr">
+        <is>
+          <t>2025-09-19 12:50:13</t>
+        </is>
+      </c>
+      <c r="M411" t="inlineStr">
+        <is>
+          <t>2025-09-19</t>
+        </is>
+      </c>
+      <c r="N411" t="inlineStr">
+        <is>
+          <t>Blocked</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>Henry Chelegbor</t>
+        </is>
+      </c>
+      <c r="B412" t="n">
+        <v>13024705411</v>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>6613 Guyer Street, Philadelphia, PA, Pennsylvania</t>
+        </is>
+      </c>
+      <c r="D412" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="E412" t="inlineStr">
+        <is>
+          <t>6613 Guyer Street, Philadelphia, Pa, Pennsylvania</t>
+        </is>
+      </c>
+      <c r="F412" t="inlineStr"/>
+      <c r="G412" t="inlineStr"/>
+      <c r="H412" t="inlineStr"/>
+      <c r="I412" t="inlineStr"/>
+      <c r="J412" t="inlineStr"/>
+      <c r="K412" t="inlineStr">
+        <is>
+          <t>WhatsApp message already sent for this book previously</t>
+        </is>
+      </c>
+      <c r="L412" t="inlineStr">
+        <is>
+          <t>2025-09-19 12:50:14</t>
+        </is>
+      </c>
+      <c r="M412" t="inlineStr">
+        <is>
+          <t>2025-09-19</t>
+        </is>
+      </c>
+      <c r="N412" t="inlineStr">
+        <is>
+          <t>Blocked</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>Dennis Vanmeter</t>
+        </is>
+      </c>
+      <c r="B413" t="n">
+        <v>13049196111</v>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>1909 Harper Rd, Beckley, WV 25801</t>
+        </is>
+      </c>
+      <c r="D413" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="E413" t="inlineStr">
+        <is>
+          <t>1909 Harper Rd, Beckley, Wv 25801</t>
+        </is>
+      </c>
+      <c r="F413" t="inlineStr"/>
+      <c r="G413" t="inlineStr"/>
+      <c r="H413" t="inlineStr"/>
+      <c r="I413" t="inlineStr"/>
+      <c r="J413" t="inlineStr"/>
+      <c r="K413" t="inlineStr">
+        <is>
+          <t>WhatsApp message already sent for this book previously</t>
+        </is>
+      </c>
+      <c r="L413" t="inlineStr">
+        <is>
+          <t>2025-09-19 12:50:16</t>
+        </is>
+      </c>
+      <c r="M413" t="inlineStr">
+        <is>
+          <t>2025-09-19</t>
+        </is>
+      </c>
+      <c r="N413" t="inlineStr">
+        <is>
+          <t>Blocked</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>Madhukar Verma</t>
+        </is>
+      </c>
+      <c r="B414" t="n">
+        <v>2065044242</v>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>42729 Mayfair Park Ave Fremont Fremont 94538 California USA</t>
+        </is>
+      </c>
+      <c r="D414" t="inlineStr">
+        <is>
+          <t>YBB</t>
+        </is>
+      </c>
+      <c r="E414" t="inlineStr">
+        <is>
+          <t>English</t>
+        </is>
+      </c>
+      <c r="F414" t="inlineStr"/>
+      <c r="G414" t="inlineStr"/>
+      <c r="H414" t="inlineStr"/>
+      <c r="I414" t="inlineStr"/>
+      <c r="J414" t="inlineStr"/>
+      <c r="K414" t="inlineStr">
+        <is>
+          <t>Same book already sent</t>
+        </is>
+      </c>
+      <c r="L414" t="inlineStr">
+        <is>
+          <t>2025-09-19 12:53:09</t>
+        </is>
+      </c>
+      <c r="M414" t="inlineStr">
+        <is>
+          <t>2025-09-19</t>
+        </is>
+      </c>
+      <c r="N414" t="inlineStr">
+        <is>
+          <t>Blocked</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>David</t>
+        </is>
+      </c>
+      <c r="B415" t="n">
+        <v>12814104622</v>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>PO Box 87301, Park Place, Houston, Texas</t>
+        </is>
+      </c>
+      <c r="D415" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="E415" t="inlineStr">
+        <is>
+          <t>Po Box 87301, Park Place, Houston, Texas</t>
+        </is>
+      </c>
+      <c r="F415" t="inlineStr"/>
+      <c r="G415" t="inlineStr"/>
+      <c r="H415" t="inlineStr"/>
+      <c r="I415" t="inlineStr"/>
+      <c r="J415" t="inlineStr"/>
+      <c r="K415" t="inlineStr">
+        <is>
+          <t>Same book already sent</t>
+        </is>
+      </c>
+      <c r="L415" t="inlineStr">
+        <is>
+          <t>2025-09-19 12:53:12</t>
+        </is>
+      </c>
+      <c r="M415" t="inlineStr">
+        <is>
+          <t>2025-09-19</t>
+        </is>
+      </c>
+      <c r="N415" t="inlineStr">
+        <is>
+          <t>Blocked</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>Henry Chelegbor</t>
+        </is>
+      </c>
+      <c r="B416" t="n">
+        <v>13024705411</v>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>6613 Guyer Street, Philadelphia, PA, Pennsylvania</t>
+        </is>
+      </c>
+      <c r="D416" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="E416" t="inlineStr">
+        <is>
+          <t>6613 Guyer Street, Philadelphia, Pa, Pennsylvania</t>
+        </is>
+      </c>
+      <c r="F416" t="inlineStr"/>
+      <c r="G416" t="inlineStr"/>
+      <c r="H416" t="inlineStr"/>
+      <c r="I416" t="inlineStr"/>
+      <c r="J416" t="inlineStr"/>
+      <c r="K416" t="inlineStr">
+        <is>
+          <t>Same book already sent</t>
+        </is>
+      </c>
+      <c r="L416" t="inlineStr">
+        <is>
+          <t>2025-09-19 12:53:14</t>
+        </is>
+      </c>
+      <c r="M416" t="inlineStr">
+        <is>
+          <t>2025-09-19</t>
+        </is>
+      </c>
+      <c r="N416" t="inlineStr">
+        <is>
+          <t>Blocked</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>Dennis Vanmeter</t>
+        </is>
+      </c>
+      <c r="B417" t="n">
+        <v>13049196111</v>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>1909 Harper Rd, Beckley, WV 25801</t>
+        </is>
+      </c>
+      <c r="D417" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="E417" t="inlineStr">
+        <is>
+          <t>1909 Harper Rd, Beckley, Wv 25801</t>
+        </is>
+      </c>
+      <c r="F417" t="inlineStr"/>
+      <c r="G417" t="inlineStr"/>
+      <c r="H417" t="inlineStr"/>
+      <c r="I417" t="inlineStr"/>
+      <c r="J417" t="inlineStr"/>
+      <c r="K417" t="inlineStr">
+        <is>
+          <t>Same book already sent</t>
+        </is>
+      </c>
+      <c r="L417" t="inlineStr">
+        <is>
+          <t>2025-09-19 12:53:17</t>
+        </is>
+      </c>
+      <c r="M417" t="inlineStr">
+        <is>
+          <t>2025-09-19</t>
+        </is>
+      </c>
+      <c r="N417" t="inlineStr">
+        <is>
+          <t>Blocked</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>David</t>
+        </is>
+      </c>
+      <c r="B418" t="n">
+        <v>12814104622</v>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>PO Box 87301, Park Place, Houston, Texas</t>
+        </is>
+      </c>
+      <c r="D418" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="E418" t="inlineStr">
+        <is>
+          <t>Po Box 87301, Park Place, Houston, Texas</t>
+        </is>
+      </c>
+      <c r="F418" t="inlineStr"/>
+      <c r="G418" t="inlineStr"/>
+      <c r="H418" t="inlineStr"/>
+      <c r="I418" t="inlineStr"/>
+      <c r="J418" t="inlineStr"/>
+      <c r="K418" t="inlineStr">
+        <is>
+          <t>Same book already sent</t>
+        </is>
+      </c>
+      <c r="L418" t="inlineStr">
+        <is>
+          <t>2025-09-19 12:53:49</t>
+        </is>
+      </c>
+      <c r="M418" t="inlineStr">
+        <is>
+          <t>2025-09-19</t>
+        </is>
+      </c>
+      <c r="N418" t="inlineStr">
+        <is>
+          <t>Blocked</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>Henry Chelegbor</t>
+        </is>
+      </c>
+      <c r="B419" t="n">
+        <v>13024705411</v>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>6613 Guyer Street, Philadelphia, PA, Pennsylvania</t>
+        </is>
+      </c>
+      <c r="D419" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="E419" t="inlineStr">
+        <is>
+          <t>6613 Guyer Street, Philadelphia, Pa, Pennsylvania</t>
+        </is>
+      </c>
+      <c r="F419" t="inlineStr"/>
+      <c r="G419" t="inlineStr"/>
+      <c r="H419" t="inlineStr"/>
+      <c r="I419" t="inlineStr"/>
+      <c r="J419" t="inlineStr"/>
+      <c r="K419" t="inlineStr">
+        <is>
+          <t>Same book already sent</t>
+        </is>
+      </c>
+      <c r="L419" t="inlineStr">
+        <is>
+          <t>2025-09-19 12:53:51</t>
+        </is>
+      </c>
+      <c r="M419" t="inlineStr">
+        <is>
+          <t>2025-09-19</t>
+        </is>
+      </c>
+      <c r="N419" t="inlineStr">
+        <is>
+          <t>Blocked</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>Dennis Vanmeter</t>
+        </is>
+      </c>
+      <c r="B420" t="n">
+        <v>13049196111</v>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>1909 Harper Rd, Beckley, WV 25801</t>
+        </is>
+      </c>
+      <c r="D420" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="E420" t="inlineStr">
+        <is>
+          <t>1909 Harper Rd, Beckley, Wv 25801</t>
+        </is>
+      </c>
+      <c r="F420" t="inlineStr"/>
+      <c r="G420" t="inlineStr"/>
+      <c r="H420" t="inlineStr"/>
+      <c r="I420" t="inlineStr"/>
+      <c r="J420" t="inlineStr"/>
+      <c r="K420" t="inlineStr">
+        <is>
+          <t>Same book already sent</t>
+        </is>
+      </c>
+      <c r="L420" t="inlineStr">
+        <is>
+          <t>2025-09-19 12:53:53</t>
+        </is>
+      </c>
+      <c r="M420" t="inlineStr">
+        <is>
+          <t>2025-09-19</t>
+        </is>
+      </c>
+      <c r="N420" t="inlineStr">
+        <is>
+          <t>Blocked</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>David</t>
+        </is>
+      </c>
+      <c r="B421" t="n">
+        <v>12814104622</v>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>PO Box 87301, Park Place, Houston, Texas</t>
+        </is>
+      </c>
+      <c r="D421" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="E421" t="inlineStr">
+        <is>
+          <t>Po Box 87301, Park Place, Houston, Texas</t>
+        </is>
+      </c>
+      <c r="F421" t="inlineStr"/>
+      <c r="G421" t="inlineStr"/>
+      <c r="H421" t="inlineStr"/>
+      <c r="I421" t="inlineStr"/>
+      <c r="J421" t="inlineStr"/>
+      <c r="K421" t="inlineStr">
+        <is>
+          <t>Same book already sent</t>
+        </is>
+      </c>
+      <c r="L421" t="inlineStr">
+        <is>
+          <t>2025-09-19 12:59:03</t>
+        </is>
+      </c>
+      <c r="M421" t="inlineStr">
+        <is>
+          <t>2025-09-19</t>
+        </is>
+      </c>
+      <c r="N421" t="inlineStr">
+        <is>
+          <t>Blocked</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>Henry Chelegbor</t>
+        </is>
+      </c>
+      <c r="B422" t="n">
+        <v>13024705411</v>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>6613 Guyer Street, Philadelphia, PA, Pennsylvania</t>
+        </is>
+      </c>
+      <c r="D422" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="E422" t="inlineStr">
+        <is>
+          <t>6613 Guyer Street, Philadelphia, Pa, Pennsylvania</t>
+        </is>
+      </c>
+      <c r="F422" t="inlineStr"/>
+      <c r="G422" t="inlineStr"/>
+      <c r="H422" t="inlineStr"/>
+      <c r="I422" t="inlineStr"/>
+      <c r="J422" t="inlineStr"/>
+      <c r="K422" t="inlineStr">
+        <is>
+          <t>Same book already sent</t>
+        </is>
+      </c>
+      <c r="L422" t="inlineStr">
+        <is>
+          <t>2025-09-19 12:59:05</t>
+        </is>
+      </c>
+      <c r="M422" t="inlineStr">
+        <is>
+          <t>2025-09-19</t>
+        </is>
+      </c>
+      <c r="N422" t="inlineStr">
+        <is>
+          <t>Blocked</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>Dennis Vanmeter</t>
+        </is>
+      </c>
+      <c r="B423" t="n">
+        <v>13049196111</v>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>1909 Harper Rd, Beckley, WV 25801</t>
+        </is>
+      </c>
+      <c r="D423" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="E423" t="inlineStr">
+        <is>
+          <t>1909 Harper Rd, Beckley, Wv 25801</t>
+        </is>
+      </c>
+      <c r="F423" t="inlineStr"/>
+      <c r="G423" t="inlineStr"/>
+      <c r="H423" t="inlineStr"/>
+      <c r="I423" t="inlineStr"/>
+      <c r="J423" t="inlineStr"/>
+      <c r="K423" t="inlineStr">
+        <is>
+          <t>Same book already sent</t>
+        </is>
+      </c>
+      <c r="L423" t="inlineStr">
+        <is>
+          <t>2025-09-19 12:59:07</t>
+        </is>
+      </c>
+      <c r="M423" t="inlineStr">
+        <is>
+          <t>2025-09-19</t>
+        </is>
+      </c>
+      <c r="N423" t="inlineStr">
+        <is>
+          <t>Blocked</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>David</t>
+        </is>
+      </c>
+      <c r="B424" t="n">
+        <v>12814104622</v>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>PO Box 87301, Park Place, Houston, Texas</t>
+        </is>
+      </c>
+      <c r="D424" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="E424" t="inlineStr">
+        <is>
+          <t>Po Box 87301, Park Place, Houston, Texas</t>
+        </is>
+      </c>
+      <c r="F424" t="inlineStr"/>
+      <c r="G424" t="inlineStr"/>
+      <c r="H424" t="inlineStr"/>
+      <c r="I424" t="inlineStr"/>
+      <c r="J424" t="inlineStr"/>
+      <c r="K424" t="inlineStr">
+        <is>
+          <t>Same book already sent</t>
+        </is>
+      </c>
+      <c r="L424" t="inlineStr">
+        <is>
+          <t>2025-09-19 13:00:34</t>
+        </is>
+      </c>
+      <c r="M424" t="inlineStr">
+        <is>
+          <t>2025-09-19</t>
+        </is>
+      </c>
+      <c r="N424" t="inlineStr">
+        <is>
+          <t>Blocked</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>Henry Chelegbor</t>
+        </is>
+      </c>
+      <c r="B425" t="n">
+        <v>13024705411</v>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>6613 Guyer Street, Philadelphia, PA, Pennsylvania</t>
+        </is>
+      </c>
+      <c r="D425" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="E425" t="inlineStr">
+        <is>
+          <t>6613 Guyer Street, Philadelphia, Pa, Pennsylvania</t>
+        </is>
+      </c>
+      <c r="F425" t="inlineStr"/>
+      <c r="G425" t="inlineStr"/>
+      <c r="H425" t="inlineStr"/>
+      <c r="I425" t="inlineStr"/>
+      <c r="J425" t="inlineStr"/>
+      <c r="K425" t="inlineStr">
+        <is>
+          <t>Same book already sent</t>
+        </is>
+      </c>
+      <c r="L425" t="inlineStr">
+        <is>
+          <t>2025-09-19 13:00:36</t>
+        </is>
+      </c>
+      <c r="M425" t="inlineStr">
+        <is>
+          <t>2025-09-19</t>
+        </is>
+      </c>
+      <c r="N425" t="inlineStr">
+        <is>
+          <t>Blocked</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>Dennis Vanmeter</t>
+        </is>
+      </c>
+      <c r="B426" t="n">
+        <v>13049196111</v>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>1909 Harper Rd, Beckley, WV 25801</t>
+        </is>
+      </c>
+      <c r="D426" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="E426" t="inlineStr">
+        <is>
+          <t>1909 Harper Rd, Beckley, Wv 25801</t>
+        </is>
+      </c>
+      <c r="F426" t="inlineStr"/>
+      <c r="G426" t="inlineStr"/>
+      <c r="H426" t="inlineStr"/>
+      <c r="I426" t="inlineStr"/>
+      <c r="J426" t="inlineStr"/>
+      <c r="K426" t="inlineStr">
+        <is>
+          <t>Same book already sent</t>
+        </is>
+      </c>
+      <c r="L426" t="inlineStr">
+        <is>
+          <t>2025-09-19 13:00:39</t>
+        </is>
+      </c>
+      <c r="M426" t="inlineStr">
+        <is>
+          <t>2025-09-19</t>
+        </is>
+      </c>
+      <c r="N426" t="inlineStr">
+        <is>
+          <t>Blocked</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>David</t>
+        </is>
+      </c>
+      <c r="B427" t="n">
+        <v>12814104622</v>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>PO Box 87301, Park Place, Houston, Texas</t>
+        </is>
+      </c>
+      <c r="D427" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="E427" t="inlineStr">
+        <is>
+          <t>Po Box 87301, Park Place, Houston, Texas</t>
+        </is>
+      </c>
+      <c r="F427" t="inlineStr"/>
+      <c r="G427" t="inlineStr"/>
+      <c r="H427" t="inlineStr"/>
+      <c r="I427" t="inlineStr"/>
+      <c r="J427" t="inlineStr"/>
+      <c r="K427" t="inlineStr">
+        <is>
+          <t>WhatsApp message already sent for this book previously</t>
+        </is>
+      </c>
+      <c r="L427" t="inlineStr">
+        <is>
+          <t>2025-09-19 13:04:39</t>
+        </is>
+      </c>
+      <c r="M427" t="inlineStr">
+        <is>
+          <t>2025-09-19</t>
+        </is>
+      </c>
+      <c r="N427" t="inlineStr">
+        <is>
+          <t>Blocked</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>Henry Chelegbor</t>
+        </is>
+      </c>
+      <c r="B428" t="n">
+        <v>13024705411</v>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>6613 Guyer Street, Philadelphia, PA, Pennsylvania</t>
+        </is>
+      </c>
+      <c r="D428" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="E428" t="inlineStr">
+        <is>
+          <t>6613 Guyer Street, Philadelphia, Pa, Pennsylvania</t>
+        </is>
+      </c>
+      <c r="F428" t="inlineStr"/>
+      <c r="G428" t="inlineStr"/>
+      <c r="H428" t="inlineStr"/>
+      <c r="I428" t="inlineStr"/>
+      <c r="J428" t="inlineStr"/>
+      <c r="K428" t="inlineStr">
+        <is>
+          <t>WhatsApp message already sent for this book previously</t>
+        </is>
+      </c>
+      <c r="L428" t="inlineStr">
+        <is>
+          <t>2025-09-19 13:04:41</t>
+        </is>
+      </c>
+      <c r="M428" t="inlineStr">
+        <is>
+          <t>2025-09-19</t>
+        </is>
+      </c>
+      <c r="N428" t="inlineStr">
+        <is>
+          <t>Blocked</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>Dennis Vanmeter</t>
+        </is>
+      </c>
+      <c r="B429" t="n">
+        <v>13049196111</v>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>1909 Harper Rd, Beckley, WV 25801</t>
+        </is>
+      </c>
+      <c r="D429" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="E429" t="inlineStr">
+        <is>
+          <t>1909 Harper Rd, Beckley, Wv 25801</t>
+        </is>
+      </c>
+      <c r="F429" t="inlineStr"/>
+      <c r="G429" t="inlineStr"/>
+      <c r="H429" t="inlineStr"/>
+      <c r="I429" t="inlineStr"/>
+      <c r="J429" t="inlineStr"/>
+      <c r="K429" t="inlineStr">
+        <is>
+          <t>WhatsApp message already sent for this book previously</t>
+        </is>
+      </c>
+      <c r="L429" t="inlineStr">
+        <is>
+          <t>2025-09-19 13:04:43</t>
+        </is>
+      </c>
+      <c r="M429" t="inlineStr">
+        <is>
+          <t>2025-09-19</t>
+        </is>
+      </c>
+      <c r="N429" t="inlineStr">
+        <is>
+          <t>Blocked</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>David</t>
+        </is>
+      </c>
+      <c r="B430" t="n">
+        <v>12814104622</v>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>PO Box 87301, Park Place, Houston, Texas</t>
+        </is>
+      </c>
+      <c r="D430" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="E430" t="inlineStr">
+        <is>
+          <t>Po Box 87301, Park Place, Houston, Texas</t>
+        </is>
+      </c>
+      <c r="F430" t="inlineStr"/>
+      <c r="G430" t="inlineStr"/>
+      <c r="H430" t="inlineStr"/>
+      <c r="I430" t="inlineStr"/>
+      <c r="J430" t="inlineStr"/>
+      <c r="K430" t="inlineStr">
+        <is>
+          <t>Same book already sent</t>
+        </is>
+      </c>
+      <c r="L430" t="inlineStr">
+        <is>
+          <t>2025-09-19 13:05:43</t>
+        </is>
+      </c>
+      <c r="M430" t="inlineStr">
+        <is>
+          <t>2025-09-19</t>
+        </is>
+      </c>
+      <c r="N430" t="inlineStr">
+        <is>
+          <t>Blocked</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>Henry Chelegbor</t>
+        </is>
+      </c>
+      <c r="B431" t="n">
+        <v>13024705411</v>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>6613 Guyer Street, Philadelphia, PA, Pennsylvania</t>
+        </is>
+      </c>
+      <c r="D431" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="E431" t="inlineStr">
+        <is>
+          <t>6613 Guyer Street, Philadelphia, Pa, Pennsylvania</t>
+        </is>
+      </c>
+      <c r="F431" t="inlineStr"/>
+      <c r="G431" t="inlineStr"/>
+      <c r="H431" t="inlineStr"/>
+      <c r="I431" t="inlineStr"/>
+      <c r="J431" t="inlineStr"/>
+      <c r="K431" t="inlineStr">
+        <is>
+          <t>Same book already sent</t>
+        </is>
+      </c>
+      <c r="L431" t="inlineStr">
+        <is>
+          <t>2025-09-19 13:05:45</t>
+        </is>
+      </c>
+      <c r="M431" t="inlineStr">
+        <is>
+          <t>2025-09-19</t>
+        </is>
+      </c>
+      <c r="N431" t="inlineStr">
+        <is>
+          <t>Blocked</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>Dennis Vanmeter</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>13049196111</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>1909 Harper Rd, Beckley, WV 25801</t>
+        </is>
+      </c>
+      <c r="D432" t="inlineStr">
+        <is>
+          <t>GG</t>
+        </is>
+      </c>
+      <c r="E432" t="inlineStr">
+        <is>
+          <t>1909 Harper Rd, Beckley, Wv 25801</t>
+        </is>
+      </c>
+      <c r="F432" t="inlineStr"/>
+      <c r="G432" t="inlineStr"/>
+      <c r="H432" t="inlineStr"/>
+      <c r="I432" t="inlineStr"/>
+      <c r="J432" t="inlineStr"/>
+      <c r="K432" t="inlineStr">
+        <is>
+          <t>Same book already sent</t>
+        </is>
+      </c>
+      <c r="L432" t="inlineStr">
+        <is>
+          <t>2025-09-19 13:05:47</t>
+        </is>
+      </c>
+      <c r="M432" t="inlineStr">
+        <is>
+          <t>2025-09-19</t>
+        </is>
+      </c>
+      <c r="N432" t="inlineStr">
+        <is>
+          <t>Blocked</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>